<commit_message>
* Hand-tuned PLL seems working. No data output, though.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Fin</t>
   </si>
@@ -60,13 +60,52 @@
   </si>
   <si>
     <t>LRClk</t>
+  </si>
+  <si>
+    <t>PLL</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>PLLCK</t>
+  </si>
+  <si>
+    <t>Fs ref</t>
+  </si>
+  <si>
+    <t>0x25 div</t>
+  </si>
+  <si>
+    <t>0x26 div</t>
+  </si>
+  <si>
+    <t>0x2A R</t>
+  </si>
+  <si>
+    <t>0x29 P</t>
+  </si>
+  <si>
+    <t>BCK</t>
+  </si>
+  <si>
+    <t>0x27 div</t>
+  </si>
+  <si>
+    <t>LRCK</t>
+  </si>
+  <si>
+    <t>BCK/Fs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +148,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +182,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -177,21 +229,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -474,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +637,132 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4">
+        <f>B14*B15*B16/B17</f>
+        <v>96000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B19/B18</f>
+        <v>46.875</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4">
+        <f>B19/(B22*B23)</f>
+        <v>3000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4">
+        <f>B19/(B22*B23*B25)</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4">
+        <f>B24/B20</f>
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hand-tuned PLL works somehow, and output produced. Wrong fs, though.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Fin</t>
   </si>
@@ -99,6 +100,18 @@
   </si>
   <si>
     <t>BCK/Fs</t>
+  </si>
+  <si>
+    <t>0x21 DSP1</t>
+  </si>
+  <si>
+    <t>0x22 DSP2</t>
+  </si>
+  <si>
+    <t>0x23 ADC</t>
+  </si>
+  <si>
+    <t>Freq, kHz</t>
   </si>
 </sst>
 </file>
@@ -190,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -228,6 +241,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -237,13 +340,22 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -529,13 +641,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -553,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>128</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,7 +685,7 @@
       </c>
       <c r="B4" s="2">
         <f>B1*B2/B3</f>
-        <v>51.2</v>
+        <v>76.8</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -598,7 +713,7 @@
       </c>
       <c r="B7" s="4">
         <f>B4*1000/((16*2)*((2*B5)+B6)*8)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -610,7 +725,7 @@
       </c>
       <c r="B8" s="4">
         <f>B7*256</f>
-        <v>2048</v>
+        <v>3072</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -622,7 +737,7 @@
       </c>
       <c r="B9">
         <f>B7*2*16</f>
-        <v>256</v>
+        <v>384</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -634,7 +749,7 @@
       </c>
       <c r="B10">
         <f>B7*2</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -666,10 +781,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.1920000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -677,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -685,82 +800,119 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="4">
         <f>B14*B15*B16/B17</f>
-        <v>96000</v>
+        <v>65536</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="4">
         <f>B19/B18</f>
-        <v>46.875</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="10">
+        <v>16</v>
+      </c>
+      <c r="G22" s="11">
+        <f>B19/F22</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="10">
+        <v>16</v>
+      </c>
+      <c r="G23" s="11">
+        <f>B19/F23</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4">
         <f>B19/(B22*B23)</f>
-        <v>3000</v>
+        <v>4096</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="13">
+        <v>32</v>
+      </c>
+      <c r="G24" s="14">
+        <f>B19/F24</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="4">
         <f>B19/(B22*B23*B25)</f>
-        <v>46.875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="4">
         <f>B24/B20</f>
-        <v>64</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Lvl Meter switched to moving average Currently no Automatic Gain Control
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -643,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +780,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>8.1920000000000002</v>
+        <v>4.0960000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -797,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>2048</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,7 +805,7 @@
       </c>
       <c r="B19" s="4">
         <f>B14*B15*B16/B17</f>
-        <v>65536</v>
+        <v>32768</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -818,7 +817,7 @@
       </c>
       <c r="B20" s="4">
         <f>B19/B18</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -842,7 +841,7 @@
         <v>25</v>
       </c>
       <c r="F22" s="10">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G22" s="11">
         <f>B19/F22</f>
@@ -864,7 +863,7 @@
       </c>
       <c r="G23" s="11">
         <f>B19/F23</f>
-        <v>4096</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,7 +872,7 @@
       </c>
       <c r="B24" s="4">
         <f>B19/(B22*B23)</f>
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -886,7 +885,7 @@
       </c>
       <c r="G24" s="14">
         <f>B19/F24</f>
-        <v>2048</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -903,7 +902,7 @@
       </c>
       <c r="B26" s="4">
         <f>B19/(B22*B23*B25)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -912,7 +911,7 @@
       </c>
       <c r="B27" s="4">
         <f>B24/B20</f>
-        <v>128</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>